<commit_message>
-works with 2019 year IEA data
</commit_message>
<xml_diff>
--- a/input/energy/EIA_Table_10.2a_Renewable_Energy_Consumption___Residential_and_Commercial_Sectors.xlsx
+++ b/input/energy/EIA_Table_10.2a_Renewable_Energy_Consumption___Residential_and_Commercial_Sectors.xlsx
@@ -21,13 +21,13 @@
     <t>U.S. Energy Information Administration</t>
   </si>
   <si>
-    <t>January 2020 Monthly Energy Review</t>
+    <t>January 2022 Monthly Energy Review</t>
   </si>
   <si>
-    <t>Release Date: January 28, 2020</t>
+    <t>Release Date: January 27, 2022</t>
   </si>
   <si>
-    <t>Next Update: February 25, 2020</t>
+    <t>Next Update: February 24, 2022</t>
   </si>
   <si>
     <t>Table 10.2a Renewable Energy Consumption:  Residential and Commercial Sectors</t>
@@ -494,7 +494,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N574"/>
+  <dimension ref="A1:N598"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -22335,7 +22335,7 @@
         <v>3.038</v>
       </c>
       <c r="C506">
-        <v>6.318</v>
+        <v>6.319</v>
       </c>
       <c r="D506">
         <v>44.381</v>
@@ -22379,13 +22379,13 @@
         <v>3.363</v>
       </c>
       <c r="C507">
-        <v>8.671</v>
+        <v>8.672</v>
       </c>
       <c r="D507">
         <v>49.136</v>
       </c>
       <c r="E507">
-        <v>61.17</v>
+        <v>61.171</v>
       </c>
       <c r="F507">
         <v>0.037</v>
@@ -22423,7 +22423,7 @@
         <v>3.255</v>
       </c>
       <c r="C508">
-        <v>9.486</v>
+        <v>9.487</v>
       </c>
       <c r="D508">
         <v>47.551</v>
@@ -22467,13 +22467,13 @@
         <v>3.363</v>
       </c>
       <c r="C509">
-        <v>10.514</v>
+        <v>10.515</v>
       </c>
       <c r="D509">
         <v>49.136</v>
       </c>
       <c r="E509">
-        <v>63.013</v>
+        <v>63.014</v>
       </c>
       <c r="F509">
         <v>0.038</v>
@@ -22511,7 +22511,7 @@
         <v>3.255</v>
       </c>
       <c r="C510">
-        <v>10.656</v>
+        <v>10.657</v>
       </c>
       <c r="D510">
         <v>47.551</v>
@@ -22561,7 +22561,7 @@
         <v>49.136</v>
       </c>
       <c r="E511">
-        <v>63.653</v>
+        <v>63.654</v>
       </c>
       <c r="F511">
         <v>0.032</v>
@@ -22599,13 +22599,13 @@
         <v>3.363</v>
       </c>
       <c r="C512">
-        <v>11.106</v>
+        <v>11.107</v>
       </c>
       <c r="D512">
         <v>49.136</v>
       </c>
       <c r="E512">
-        <v>63.605</v>
+        <v>63.606</v>
       </c>
       <c r="F512">
         <v>0.026</v>
@@ -22643,13 +22643,13 @@
         <v>3.255</v>
       </c>
       <c r="C513">
-        <v>10.295</v>
+        <v>10.296</v>
       </c>
       <c r="D513">
         <v>47.551</v>
       </c>
       <c r="E513">
-        <v>61.101</v>
+        <v>61.102</v>
       </c>
       <c r="F513">
         <v>0.026</v>
@@ -22731,13 +22731,13 @@
         <v>3.255</v>
       </c>
       <c r="C515">
-        <v>7.94</v>
+        <v>7.941</v>
       </c>
       <c r="D515">
         <v>47.551</v>
       </c>
       <c r="E515">
-        <v>58.746</v>
+        <v>58.747</v>
       </c>
       <c r="F515">
         <v>0.018</v>
@@ -22819,13 +22819,13 @@
         <v>3.363</v>
       </c>
       <c r="C517">
-        <v>6.486</v>
+        <v>6.492</v>
       </c>
       <c r="D517">
         <v>43.547</v>
       </c>
       <c r="E517">
-        <v>53.396</v>
+        <v>53.402</v>
       </c>
       <c r="F517">
         <v>0.031</v>
@@ -22863,13 +22863,13 @@
         <v>3.038</v>
       </c>
       <c r="C518">
-        <v>7.119</v>
+        <v>7.126</v>
       </c>
       <c r="D518">
         <v>39.333</v>
       </c>
       <c r="E518">
-        <v>49.49</v>
+        <v>49.497</v>
       </c>
       <c r="F518">
         <v>0.024</v>
@@ -22907,13 +22907,13 @@
         <v>3.363</v>
       </c>
       <c r="C519">
-        <v>10.032</v>
+        <v>10.041</v>
       </c>
       <c r="D519">
         <v>43.547</v>
       </c>
       <c r="E519">
-        <v>56.942</v>
+        <v>56.951</v>
       </c>
       <c r="F519">
         <v>0.025</v>
@@ -22951,13 +22951,13 @@
         <v>3.255</v>
       </c>
       <c r="C520">
-        <v>11.299</v>
+        <v>11.309</v>
       </c>
       <c r="D520">
         <v>42.143</v>
       </c>
       <c r="E520">
-        <v>56.696</v>
+        <v>56.707</v>
       </c>
       <c r="F520">
         <v>0.025</v>
@@ -22995,13 +22995,13 @@
         <v>3.363</v>
       </c>
       <c r="C521">
-        <v>12.5</v>
+        <v>12.511</v>
       </c>
       <c r="D521">
         <v>43.547</v>
       </c>
       <c r="E521">
-        <v>59.411</v>
+        <v>59.422</v>
       </c>
       <c r="F521">
         <v>0.024</v>
@@ -23039,13 +23039,13 @@
         <v>3.255</v>
       </c>
       <c r="C522">
-        <v>12.721</v>
+        <v>12.733</v>
       </c>
       <c r="D522">
         <v>42.143</v>
       </c>
       <c r="E522">
-        <v>58.119</v>
+        <v>58.13</v>
       </c>
       <c r="F522">
         <v>0.033</v>
@@ -23083,13 +23083,13 @@
         <v>3.363</v>
       </c>
       <c r="C523">
-        <v>13.514</v>
+        <v>13.526</v>
       </c>
       <c r="D523">
         <v>43.547</v>
       </c>
       <c r="E523">
-        <v>60.425</v>
+        <v>60.437</v>
       </c>
       <c r="F523">
         <v>0.029</v>
@@ -23127,13 +23127,13 @@
         <v>3.363</v>
       </c>
       <c r="C524">
-        <v>13.477</v>
+        <v>13.489</v>
       </c>
       <c r="D524">
         <v>43.547</v>
       </c>
       <c r="E524">
-        <v>60.388</v>
+        <v>60.399</v>
       </c>
       <c r="F524">
         <v>0.023</v>
@@ -23171,13 +23171,13 @@
         <v>3.255</v>
       </c>
       <c r="C525">
-        <v>12.245</v>
+        <v>12.256</v>
       </c>
       <c r="D525">
         <v>42.143</v>
       </c>
       <c r="E525">
-        <v>57.642</v>
+        <v>57.653</v>
       </c>
       <c r="F525">
         <v>0.02</v>
@@ -23215,13 +23215,13 @@
         <v>3.363</v>
       </c>
       <c r="C526">
-        <v>11.084</v>
+        <v>11.094</v>
       </c>
       <c r="D526">
         <v>43.547</v>
       </c>
       <c r="E526">
-        <v>57.995</v>
+        <v>58.004</v>
       </c>
       <c r="F526">
         <v>0.026</v>
@@ -23259,13 +23259,13 @@
         <v>3.255</v>
       </c>
       <c r="C527">
-        <v>9.165</v>
+        <v>9.173</v>
       </c>
       <c r="D527">
         <v>42.143</v>
       </c>
       <c r="E527">
-        <v>54.562</v>
+        <v>54.57</v>
       </c>
       <c r="F527">
         <v>0.027</v>
@@ -23303,13 +23303,13 @@
         <v>3.363</v>
       </c>
       <c r="C528">
-        <v>8.457</v>
+        <v>8.465</v>
       </c>
       <c r="D528">
         <v>43.547</v>
       </c>
       <c r="E528">
-        <v>55.368</v>
+        <v>55.375</v>
       </c>
       <c r="F528">
         <v>0.039</v>
@@ -23347,13 +23347,13 @@
         <v>3.354</v>
       </c>
       <c r="C529">
-        <v>8.106</v>
+        <v>8.116</v>
       </c>
       <c r="D529">
-        <v>37.932</v>
+        <v>37.654</v>
       </c>
       <c r="E529">
-        <v>49.391</v>
+        <v>49.124</v>
       </c>
       <c r="F529">
         <v>0.195</v>
@@ -23391,13 +23391,13 @@
         <v>3.138</v>
       </c>
       <c r="C530">
-        <v>9.603</v>
+        <v>9.616</v>
       </c>
       <c r="D530">
-        <v>35.485</v>
+        <v>35.224</v>
       </c>
       <c r="E530">
-        <v>48.225</v>
+        <v>47.978</v>
       </c>
       <c r="F530">
         <v>0.164</v>
@@ -23435,13 +23435,13 @@
         <v>3.354</v>
       </c>
       <c r="C531">
-        <v>12.851</v>
+        <v>12.868</v>
       </c>
       <c r="D531">
-        <v>37.932</v>
+        <v>37.654</v>
       </c>
       <c r="E531">
-        <v>54.137</v>
+        <v>53.876</v>
       </c>
       <c r="F531">
         <v>0.204</v>
@@ -23479,13 +23479,13 @@
         <v>3.246</v>
       </c>
       <c r="C532">
-        <v>14.526</v>
+        <v>14.545</v>
       </c>
       <c r="D532">
-        <v>36.708</v>
+        <v>36.439</v>
       </c>
       <c r="E532">
-        <v>54.48</v>
+        <v>54.23</v>
       </c>
       <c r="F532">
         <v>0.135</v>
@@ -23523,13 +23523,13 @@
         <v>3.354</v>
       </c>
       <c r="C533">
-        <v>16.105</v>
+        <v>16.125</v>
       </c>
       <c r="D533">
-        <v>37.932</v>
+        <v>37.654</v>
       </c>
       <c r="E533">
-        <v>57.39</v>
+        <v>57.133</v>
       </c>
       <c r="F533">
         <v>0.106</v>
@@ -23567,13 +23567,13 @@
         <v>3.246</v>
       </c>
       <c r="C534">
-        <v>16.651</v>
+        <v>16.672</v>
       </c>
       <c r="D534">
-        <v>36.708</v>
+        <v>36.439</v>
       </c>
       <c r="E534">
-        <v>56.605</v>
+        <v>56.357</v>
       </c>
       <c r="F534">
         <v>0.118</v>
@@ -23611,13 +23611,13 @@
         <v>3.354</v>
       </c>
       <c r="C535">
-        <v>17.333</v>
+        <v>17.356</v>
       </c>
       <c r="D535">
-        <v>37.932</v>
+        <v>37.654</v>
       </c>
       <c r="E535">
-        <v>58.619</v>
+        <v>58.363</v>
       </c>
       <c r="F535">
         <v>0.138</v>
@@ -23655,13 +23655,13 @@
         <v>3.354</v>
       </c>
       <c r="C536">
-        <v>16.825</v>
+        <v>16.847</v>
       </c>
       <c r="D536">
-        <v>37.932</v>
+        <v>37.654</v>
       </c>
       <c r="E536">
-        <v>58.111</v>
+        <v>57.855</v>
       </c>
       <c r="F536">
         <v>0.177</v>
@@ -23699,13 +23699,13 @@
         <v>3.246</v>
       </c>
       <c r="C537">
-        <v>14.987</v>
+        <v>15.007</v>
       </c>
       <c r="D537">
-        <v>36.708</v>
+        <v>36.439</v>
       </c>
       <c r="E537">
-        <v>54.941</v>
+        <v>54.692</v>
       </c>
       <c r="F537">
         <v>0.217</v>
@@ -23743,13 +23743,13 @@
         <v>3.354</v>
       </c>
       <c r="C538">
-        <v>13.402</v>
+        <v>13.419</v>
       </c>
       <c r="D538">
-        <v>37.932</v>
+        <v>37.654</v>
       </c>
       <c r="E538">
-        <v>54.688</v>
+        <v>54.427</v>
       </c>
       <c r="F538">
         <v>0.198</v>
@@ -23787,13 +23787,13 @@
         <v>3.246</v>
       </c>
       <c r="C539">
-        <v>10.941</v>
+        <v>10.955</v>
       </c>
       <c r="D539">
-        <v>36.708</v>
+        <v>36.439</v>
       </c>
       <c r="E539">
-        <v>50.895</v>
+        <v>50.64</v>
       </c>
       <c r="F539">
         <v>0.161</v>
@@ -23831,13 +23831,13 @@
         <v>3.354</v>
       </c>
       <c r="C540">
-        <v>9.963</v>
+        <v>9.976</v>
       </c>
       <c r="D540">
-        <v>37.932</v>
+        <v>37.654</v>
       </c>
       <c r="E540">
-        <v>51.249</v>
+        <v>50.983</v>
       </c>
       <c r="F540">
         <v>0.191</v>
@@ -23875,25 +23875,25 @@
         <v>3.363</v>
       </c>
       <c r="C541">
-        <v>9.849</v>
+        <v>9.85</v>
       </c>
       <c r="D541">
-        <v>36.775</v>
+        <v>36.452</v>
       </c>
       <c r="E541">
-        <v>49.987</v>
+        <v>49.666</v>
       </c>
       <c r="F541">
-        <v>0.251</v>
+        <v>0.197</v>
       </c>
       <c r="G541">
         <v>1.673</v>
       </c>
       <c r="H541">
-        <v>4.033</v>
+        <v>4.095</v>
       </c>
       <c r="I541">
-        <v>0.1</v>
+        <v>0.104</v>
       </c>
       <c r="J541">
         <v>7.269</v>
@@ -23908,7 +23908,7 @@
         <v>13.532</v>
       </c>
       <c r="N541">
-        <v>19.59</v>
+        <v>19.602</v>
       </c>
     </row>
     <row r="542" spans="1:14">
@@ -23919,40 +23919,40 @@
         <v>3.038</v>
       </c>
       <c r="C542">
-        <v>11.02</v>
+        <v>11.022</v>
       </c>
       <c r="D542">
-        <v>33.216</v>
+        <v>32.925</v>
       </c>
       <c r="E542">
-        <v>47.274</v>
+        <v>46.984</v>
       </c>
       <c r="F542">
-        <v>0.141</v>
+        <v>0.182</v>
       </c>
       <c r="G542">
         <v>1.511</v>
       </c>
       <c r="H542">
-        <v>4.465</v>
+        <v>4.516</v>
       </c>
       <c r="I542">
-        <v>0.097</v>
+        <v>0.101</v>
       </c>
       <c r="J542">
         <v>6.521</v>
       </c>
       <c r="K542">
-        <v>3.769</v>
+        <v>3.792</v>
       </c>
       <c r="L542">
         <v>1.835</v>
       </c>
       <c r="M542">
-        <v>12.124</v>
+        <v>12.147</v>
       </c>
       <c r="N542">
-        <v>18.338</v>
+        <v>18.457</v>
       </c>
     </row>
     <row r="543" spans="1:14">
@@ -23963,40 +23963,40 @@
         <v>3.363</v>
       </c>
       <c r="C543">
-        <v>15.904</v>
+        <v>15.906</v>
       </c>
       <c r="D543">
-        <v>36.775</v>
+        <v>36.452</v>
       </c>
       <c r="E543">
-        <v>56.042</v>
+        <v>55.722</v>
       </c>
       <c r="F543">
-        <v>0.136</v>
+        <v>0.223</v>
       </c>
       <c r="G543">
         <v>1.673</v>
       </c>
       <c r="H543">
-        <v>6.185</v>
+        <v>6.225</v>
       </c>
       <c r="I543">
-        <v>0.151</v>
+        <v>0.153</v>
       </c>
       <c r="J543">
         <v>7.013</v>
       </c>
       <c r="K543">
-        <v>4.002</v>
+        <v>4.006</v>
       </c>
       <c r="L543">
         <v>2.082</v>
       </c>
       <c r="M543">
-        <v>13.097</v>
+        <v>13.101</v>
       </c>
       <c r="N543">
-        <v>21.241</v>
+        <v>21.376</v>
       </c>
     </row>
     <row r="544" spans="1:14">
@@ -24007,40 +24007,40 @@
         <v>3.255</v>
       </c>
       <c r="C544">
-        <v>17.764</v>
+        <v>17.766</v>
       </c>
       <c r="D544">
-        <v>35.588</v>
+        <v>35.277</v>
       </c>
       <c r="E544">
-        <v>56.607</v>
+        <v>56.298</v>
       </c>
       <c r="F544">
-        <v>0.209</v>
+        <v>0.234</v>
       </c>
       <c r="G544">
         <v>1.619</v>
       </c>
       <c r="H544">
-        <v>6.859</v>
+        <v>6.894</v>
       </c>
       <c r="I544">
-        <v>0.135</v>
+        <v>0.136</v>
       </c>
       <c r="J544">
         <v>6.801</v>
       </c>
       <c r="K544">
-        <v>3.891</v>
+        <v>3.894</v>
       </c>
       <c r="L544">
         <v>2.042</v>
       </c>
       <c r="M544">
-        <v>12.734</v>
+        <v>12.737</v>
       </c>
       <c r="N544">
-        <v>21.556</v>
+        <v>21.62</v>
       </c>
     </row>
     <row r="545" spans="1:14">
@@ -24051,40 +24051,40 @@
         <v>3.363</v>
       </c>
       <c r="C545">
-        <v>19.594</v>
+        <v>19.598</v>
       </c>
       <c r="D545">
-        <v>36.775</v>
+        <v>36.452</v>
       </c>
       <c r="E545">
-        <v>59.732</v>
+        <v>59.413</v>
       </c>
       <c r="F545">
-        <v>0.224</v>
+        <v>0.25</v>
       </c>
       <c r="G545">
         <v>1.673</v>
       </c>
       <c r="H545">
-        <v>7.583</v>
+        <v>7.606</v>
       </c>
       <c r="I545">
-        <v>0.12</v>
+        <v>0.121</v>
       </c>
       <c r="J545">
         <v>7.032</v>
       </c>
       <c r="K545">
-        <v>4.072</v>
+        <v>4.049</v>
       </c>
       <c r="L545">
         <v>2.176</v>
       </c>
       <c r="M545">
-        <v>13.28</v>
+        <v>13.257</v>
       </c>
       <c r="N545">
-        <v>22.881</v>
+        <v>22.908</v>
       </c>
     </row>
     <row r="546" spans="1:14">
@@ -24095,22 +24095,22 @@
         <v>3.255</v>
       </c>
       <c r="C546">
-        <v>20.263</v>
+        <v>20.266</v>
       </c>
       <c r="D546">
-        <v>35.588</v>
+        <v>35.277</v>
       </c>
       <c r="E546">
-        <v>59.106</v>
+        <v>58.798</v>
       </c>
       <c r="F546">
-        <v>0.141</v>
+        <v>0.223</v>
       </c>
       <c r="G546">
         <v>1.619</v>
       </c>
       <c r="H546">
-        <v>7.719</v>
+        <v>7.696</v>
       </c>
       <c r="I546">
         <v>0.098</v>
@@ -24119,16 +24119,16 @@
         <v>6.832</v>
       </c>
       <c r="K546">
-        <v>3.954</v>
+        <v>3.955</v>
       </c>
       <c r="L546">
         <v>2.175</v>
       </c>
       <c r="M546">
-        <v>12.961</v>
+        <v>12.963</v>
       </c>
       <c r="N546">
-        <v>22.538</v>
+        <v>22.598</v>
       </c>
     </row>
     <row r="547" spans="1:14">
@@ -24139,22 +24139,22 @@
         <v>3.363</v>
       </c>
       <c r="C547">
-        <v>20.686</v>
+        <v>20.69</v>
       </c>
       <c r="D547">
-        <v>36.775</v>
+        <v>36.452</v>
       </c>
       <c r="E547">
-        <v>60.824</v>
+        <v>60.505</v>
       </c>
       <c r="F547">
-        <v>0.129</v>
+        <v>0.195</v>
       </c>
       <c r="G547">
         <v>1.673</v>
       </c>
       <c r="H547">
-        <v>7.98</v>
+        <v>7.948</v>
       </c>
       <c r="I547">
         <v>0.074</v>
@@ -24163,16 +24163,16 @@
         <v>7.083</v>
       </c>
       <c r="K547">
-        <v>4.094</v>
+        <v>4.095</v>
       </c>
       <c r="L547">
         <v>2.146</v>
       </c>
       <c r="M547">
-        <v>13.324</v>
+        <v>13.325</v>
       </c>
       <c r="N547">
-        <v>23.18</v>
+        <v>23.215</v>
       </c>
     </row>
     <row r="548" spans="1:14">
@@ -24183,22 +24183,22 @@
         <v>3.363</v>
       </c>
       <c r="C548">
-        <v>20.033</v>
+        <v>20.036</v>
       </c>
       <c r="D548">
-        <v>36.775</v>
+        <v>36.452</v>
       </c>
       <c r="E548">
-        <v>60.171</v>
+        <v>59.852</v>
       </c>
       <c r="F548">
-        <v>0.158</v>
+        <v>0.162</v>
       </c>
       <c r="G548">
         <v>1.673</v>
       </c>
       <c r="H548">
-        <v>7.766</v>
+        <v>7.746</v>
       </c>
       <c r="I548">
         <v>0.053</v>
@@ -24207,16 +24207,16 @@
         <v>7.094</v>
       </c>
       <c r="K548">
-        <v>4.091</v>
+        <v>4.11</v>
       </c>
       <c r="L548">
         <v>2.233</v>
       </c>
       <c r="M548">
-        <v>13.417</v>
+        <v>13.437</v>
       </c>
       <c r="N548">
-        <v>23.068</v>
+        <v>23.071</v>
       </c>
     </row>
     <row r="549" spans="1:14">
@@ -24227,40 +24227,40 @@
         <v>3.255</v>
       </c>
       <c r="C549">
-        <v>17.939</v>
+        <v>17.942</v>
       </c>
       <c r="D549">
-        <v>35.588</v>
+        <v>35.277</v>
       </c>
       <c r="E549">
-        <v>56.782</v>
+        <v>56.473</v>
       </c>
       <c r="F549">
-        <v>0.131</v>
+        <v>0.14</v>
       </c>
       <c r="G549">
         <v>1.619</v>
       </c>
       <c r="H549">
-        <v>7.013</v>
+        <v>6.983</v>
       </c>
       <c r="I549">
-        <v>0.102</v>
+        <v>0.103</v>
       </c>
       <c r="J549">
         <v>6.721</v>
       </c>
       <c r="K549">
-        <v>3.685</v>
+        <v>3.679</v>
       </c>
       <c r="L549">
         <v>2.088</v>
       </c>
       <c r="M549">
-        <v>12.494</v>
+        <v>12.488</v>
       </c>
       <c r="N549">
-        <v>21.359</v>
+        <v>21.333</v>
       </c>
     </row>
     <row r="550" spans="1:14">
@@ -24271,40 +24271,40 @@
         <v>3.363</v>
       </c>
       <c r="C550">
-        <v>16.044</v>
+        <v>16.046</v>
       </c>
       <c r="D550">
-        <v>36.775</v>
+        <v>36.452</v>
       </c>
       <c r="E550">
-        <v>56.181</v>
+        <v>55.862</v>
       </c>
       <c r="F550">
-        <v>0.27</v>
+        <v>0.119</v>
       </c>
       <c r="G550">
         <v>1.673</v>
       </c>
       <c r="H550">
-        <v>6.258</v>
+        <v>6.197</v>
       </c>
       <c r="I550">
-        <v>0.139</v>
+        <v>0.137</v>
       </c>
       <c r="J550">
         <v>7.123</v>
       </c>
       <c r="K550">
-        <v>3.684</v>
+        <v>3.678</v>
       </c>
       <c r="L550">
         <v>2.163</v>
       </c>
       <c r="M550">
-        <v>12.97</v>
+        <v>12.964</v>
       </c>
       <c r="N550">
-        <v>21.31</v>
+        <v>21.09</v>
       </c>
     </row>
     <row r="551" spans="1:14">
@@ -24315,40 +24315,40 @@
         <v>3.255</v>
       </c>
       <c r="C551">
-        <v>12.552</v>
+        <v>12.554</v>
       </c>
       <c r="D551">
-        <v>35.588</v>
+        <v>35.277</v>
       </c>
       <c r="E551">
-        <v>51.395</v>
+        <v>51.085</v>
       </c>
       <c r="F551">
-        <v>0.21</v>
+        <v>0.133</v>
       </c>
       <c r="G551">
         <v>1.619</v>
       </c>
       <c r="H551">
-        <v>4.937</v>
+        <v>4.918</v>
       </c>
       <c r="I551">
-        <v>0.132</v>
+        <v>0.128</v>
       </c>
       <c r="J551">
         <v>6.986</v>
       </c>
       <c r="K551">
-        <v>3.921</v>
+        <v>3.907</v>
       </c>
       <c r="L551">
         <v>2.12</v>
       </c>
       <c r="M551">
-        <v>13.027</v>
+        <v>13.013</v>
       </c>
       <c r="N551">
-        <v>19.925</v>
+        <v>19.811</v>
       </c>
     </row>
     <row r="552" spans="1:14">
@@ -24359,40 +24359,40 @@
         <v>3.363</v>
       </c>
       <c r="C552">
-        <v>11.736</v>
+        <v>11.738</v>
       </c>
       <c r="D552">
-        <v>36.775</v>
+        <v>36.452</v>
       </c>
       <c r="E552">
-        <v>51.874</v>
+        <v>51.553</v>
       </c>
       <c r="F552">
-        <v>0.209</v>
+        <v>0.151</v>
       </c>
       <c r="G552">
         <v>1.673</v>
       </c>
       <c r="H552">
-        <v>4.803</v>
+        <v>4.777</v>
       </c>
       <c r="I552">
-        <v>0.127</v>
+        <v>0.12</v>
       </c>
       <c r="J552">
         <v>7.254</v>
       </c>
       <c r="K552">
-        <v>4.057</v>
+        <v>4.054</v>
       </c>
       <c r="L552">
         <v>2.113</v>
       </c>
       <c r="M552">
-        <v>13.424</v>
+        <v>13.422</v>
       </c>
       <c r="N552">
-        <v>20.237</v>
+        <v>20.143</v>
       </c>
     </row>
     <row r="553" spans="1:14">
@@ -24403,13 +24403,13 @@
         <v>3.363</v>
       </c>
       <c r="C553">
-        <v>11.976</v>
+        <v>11.95</v>
       </c>
       <c r="D553">
-        <v>43.93</v>
+        <v>44.534</v>
       </c>
       <c r="E553">
-        <v>59.269</v>
+        <v>59.848</v>
       </c>
       <c r="F553">
         <v>0.172</v>
@@ -24418,7 +24418,7 @@
         <v>1.673</v>
       </c>
       <c r="H553">
-        <v>5.298</v>
+        <v>5.29</v>
       </c>
       <c r="I553">
         <v>0.16</v>
@@ -24430,13 +24430,13 @@
         <v>3.987</v>
       </c>
       <c r="L553">
-        <v>2.101</v>
+        <v>2.133</v>
       </c>
       <c r="M553">
-        <v>13.293</v>
+        <v>13.325</v>
       </c>
       <c r="N553">
-        <v>20.597</v>
+        <v>20.62</v>
       </c>
     </row>
     <row r="554" spans="1:14">
@@ -24447,13 +24447,13 @@
         <v>3.038</v>
       </c>
       <c r="C554">
-        <v>13.088</v>
+        <v>13.058</v>
       </c>
       <c r="D554">
-        <v>39.678</v>
+        <v>40.224</v>
       </c>
       <c r="E554">
-        <v>55.804</v>
+        <v>56.32</v>
       </c>
       <c r="F554">
         <v>0.175</v>
@@ -24462,7 +24462,7 @@
         <v>1.511</v>
       </c>
       <c r="H554">
-        <v>5.796</v>
+        <v>5.787</v>
       </c>
       <c r="I554">
         <v>0.141</v>
@@ -24474,13 +24474,13 @@
         <v>3.709</v>
       </c>
       <c r="L554">
-        <v>1.788</v>
+        <v>1.815</v>
       </c>
       <c r="M554">
-        <v>12.054</v>
+        <v>12.081</v>
       </c>
       <c r="N554">
-        <v>19.676</v>
+        <v>19.694</v>
       </c>
     </row>
     <row r="555" spans="1:14">
@@ -24491,13 +24491,13 @@
         <v>3.363</v>
       </c>
       <c r="C555">
-        <v>18.09</v>
+        <v>18.05</v>
       </c>
       <c r="D555">
-        <v>43.93</v>
+        <v>44.534</v>
       </c>
       <c r="E555">
-        <v>65.383</v>
+        <v>65.947</v>
       </c>
       <c r="F555">
         <v>0.195</v>
@@ -24506,7 +24506,7 @@
         <v>1.673</v>
       </c>
       <c r="H555">
-        <v>7.868</v>
+        <v>7.855</v>
       </c>
       <c r="I555">
         <v>0.168</v>
@@ -24518,13 +24518,13 @@
         <v>3.987</v>
       </c>
       <c r="L555">
-        <v>2.085</v>
+        <v>2.116</v>
       </c>
       <c r="M555">
-        <v>13.288</v>
+        <v>13.319</v>
       </c>
       <c r="N555">
-        <v>23.192</v>
+        <v>23.211</v>
       </c>
     </row>
     <row r="556" spans="1:14">
@@ -24535,13 +24535,13 @@
         <v>3.255</v>
       </c>
       <c r="C556">
-        <v>20.587</v>
+        <v>20.534</v>
       </c>
       <c r="D556">
-        <v>42.513</v>
+        <v>43.098</v>
       </c>
       <c r="E556">
-        <v>66.355</v>
+        <v>66.886</v>
       </c>
       <c r="F556">
         <v>0.214</v>
@@ -24550,7 +24550,7 @@
         <v>1.619</v>
       </c>
       <c r="H556">
-        <v>8.724</v>
+        <v>8.711</v>
       </c>
       <c r="I556">
         <v>0.146</v>
@@ -24562,13 +24562,13 @@
         <v>3.899</v>
       </c>
       <c r="L556">
-        <v>1.952</v>
+        <v>1.982</v>
       </c>
       <c r="M556">
-        <v>12.679</v>
+        <v>12.709</v>
       </c>
       <c r="N556">
-        <v>23.383</v>
+        <v>23.399</v>
       </c>
     </row>
     <row r="557" spans="1:14">
@@ -24579,13 +24579,13 @@
         <v>3.363</v>
       </c>
       <c r="C557">
-        <v>22.659</v>
+        <v>22.594</v>
       </c>
       <c r="D557">
-        <v>43.93</v>
+        <v>44.534</v>
       </c>
       <c r="E557">
-        <v>69.952</v>
+        <v>70.491</v>
       </c>
       <c r="F557">
         <v>0.222</v>
@@ -24594,7 +24594,7 @@
         <v>1.673</v>
       </c>
       <c r="H557">
-        <v>9.559</v>
+        <v>9.545</v>
       </c>
       <c r="I557">
         <v>0.124</v>
@@ -24606,13 +24606,13 @@
         <v>4.041</v>
       </c>
       <c r="L557">
-        <v>2.255</v>
+        <v>2.289</v>
       </c>
       <c r="M557">
-        <v>13.335</v>
+        <v>13.369</v>
       </c>
       <c r="N557">
-        <v>24.914</v>
+        <v>24.933</v>
       </c>
     </row>
     <row r="558" spans="1:14">
@@ -24623,22 +24623,22 @@
         <v>3.255</v>
       </c>
       <c r="C558">
-        <v>23.092</v>
+        <v>23.021</v>
       </c>
       <c r="D558">
-        <v>42.513</v>
+        <v>43.098</v>
       </c>
       <c r="E558">
-        <v>68.859</v>
+        <v>69.374</v>
       </c>
       <c r="F558">
-        <v>0.193</v>
+        <v>0.192</v>
       </c>
       <c r="G558">
         <v>1.619</v>
       </c>
       <c r="H558">
-        <v>9.712</v>
+        <v>9.697</v>
       </c>
       <c r="I558">
         <v>0.125</v>
@@ -24650,13 +24650,13 @@
         <v>3.921</v>
       </c>
       <c r="L558">
-        <v>2.129</v>
+        <v>2.161</v>
       </c>
       <c r="M558">
-        <v>12.977</v>
+        <v>13.009</v>
       </c>
       <c r="N558">
-        <v>24.626</v>
+        <v>24.643</v>
       </c>
     </row>
     <row r="559" spans="1:14">
@@ -24667,13 +24667,13 @@
         <v>3.363</v>
       </c>
       <c r="C559">
-        <v>23.702</v>
+        <v>23.63</v>
       </c>
       <c r="D559">
-        <v>43.93</v>
+        <v>44.534</v>
       </c>
       <c r="E559">
-        <v>70.995</v>
+        <v>71.527</v>
       </c>
       <c r="F559">
         <v>0.173</v>
@@ -24682,7 +24682,7 @@
         <v>1.673</v>
       </c>
       <c r="H559">
-        <v>9.98</v>
+        <v>9.964</v>
       </c>
       <c r="I559">
         <v>0.088</v>
@@ -24694,13 +24694,13 @@
         <v>3.973</v>
       </c>
       <c r="L559">
-        <v>2.207</v>
+        <v>2.24</v>
       </c>
       <c r="M559">
-        <v>13.309</v>
+        <v>13.342</v>
       </c>
       <c r="N559">
-        <v>25.223</v>
+        <v>25.24</v>
       </c>
     </row>
     <row r="560" spans="1:14">
@@ -24711,13 +24711,13 @@
         <v>3.363</v>
       </c>
       <c r="C560">
-        <v>22.711</v>
+        <v>22.64</v>
       </c>
       <c r="D560">
-        <v>43.93</v>
+        <v>44.534</v>
       </c>
       <c r="E560">
-        <v>70.004</v>
+        <v>70.538</v>
       </c>
       <c r="F560">
         <v>0.159</v>
@@ -24726,7 +24726,7 @@
         <v>1.673</v>
       </c>
       <c r="H560">
-        <v>9.566</v>
+        <v>9.551</v>
       </c>
       <c r="I560">
         <v>0.099</v>
@@ -24738,13 +24738,13 @@
         <v>4.049</v>
       </c>
       <c r="L560">
-        <v>2.274</v>
+        <v>2.308</v>
       </c>
       <c r="M560">
-        <v>13.498</v>
+        <v>13.532</v>
       </c>
       <c r="N560">
-        <v>24.994</v>
+        <v>25.013</v>
       </c>
     </row>
     <row r="561" spans="1:14">
@@ -24755,13 +24755,13 @@
         <v>3.255</v>
       </c>
       <c r="C561">
-        <v>19.981</v>
+        <v>19.907</v>
       </c>
       <c r="D561">
-        <v>42.513</v>
+        <v>43.098</v>
       </c>
       <c r="E561">
-        <v>65.749</v>
+        <v>66.26</v>
       </c>
       <c r="F561">
         <v>0.142</v>
@@ -24770,10 +24770,10 @@
         <v>1.619</v>
       </c>
       <c r="H561">
-        <v>8.556</v>
+        <v>8.542</v>
       </c>
       <c r="I561">
-        <v>0.111</v>
+        <v>0.11</v>
       </c>
       <c r="J561">
         <v>6.861</v>
@@ -24782,13 +24782,13 @@
         <v>3.602</v>
       </c>
       <c r="L561">
-        <v>1.956</v>
+        <v>1.986</v>
       </c>
       <c r="M561">
-        <v>12.418</v>
+        <v>12.448</v>
       </c>
       <c r="N561">
-        <v>22.846</v>
+        <v>22.862</v>
       </c>
     </row>
     <row r="562" spans="1:14">
@@ -24799,13 +24799,13 @@
         <v>3.363</v>
       </c>
       <c r="C562">
-        <v>17.959</v>
+        <v>17.885</v>
       </c>
       <c r="D562">
-        <v>43.93</v>
+        <v>44.534</v>
       </c>
       <c r="E562">
-        <v>65.252</v>
+        <v>65.783</v>
       </c>
       <c r="F562">
         <v>0.129</v>
@@ -24814,10 +24814,10 @@
         <v>1.673</v>
       </c>
       <c r="H562">
-        <v>7.53</v>
+        <v>7.518</v>
       </c>
       <c r="I562">
-        <v>0.138</v>
+        <v>0.137</v>
       </c>
       <c r="J562">
         <v>7.044</v>
@@ -24826,13 +24826,13 @@
         <v>3.868</v>
       </c>
       <c r="L562">
-        <v>2.156</v>
+        <v>2.189</v>
       </c>
       <c r="M562">
-        <v>13.068</v>
+        <v>13.1</v>
       </c>
       <c r="N562">
-        <v>22.538</v>
+        <v>22.558</v>
       </c>
     </row>
     <row r="563" spans="1:14">
@@ -24843,13 +24843,13 @@
         <v>3.255</v>
       </c>
       <c r="C563">
-        <v>14.35</v>
+        <v>14.287</v>
       </c>
       <c r="D563">
-        <v>42.513</v>
+        <v>43.098</v>
       </c>
       <c r="E563">
-        <v>60.118</v>
+        <v>60.639</v>
       </c>
       <c r="F563">
         <v>0.145</v>
@@ -24858,7 +24858,7 @@
         <v>1.619</v>
       </c>
       <c r="H563">
-        <v>5.948</v>
+        <v>5.939</v>
       </c>
       <c r="I563">
         <v>0.147</v>
@@ -24870,13 +24870,13 @@
         <v>3.876</v>
       </c>
       <c r="L563">
-        <v>2.075</v>
+        <v>2.106</v>
       </c>
       <c r="M563">
-        <v>12.787</v>
+        <v>12.818</v>
       </c>
       <c r="N563">
-        <v>20.647</v>
+        <v>20.669</v>
       </c>
     </row>
     <row r="564" spans="1:14">
@@ -24887,22 +24887,22 @@
         <v>3.363</v>
       </c>
       <c r="C564">
-        <v>13.317</v>
+        <v>13.279</v>
       </c>
       <c r="D564">
-        <v>43.93</v>
+        <v>44.534</v>
       </c>
       <c r="E564">
-        <v>60.61</v>
+        <v>61.177</v>
       </c>
       <c r="F564">
-        <v>0.152</v>
+        <v>0.151</v>
       </c>
       <c r="G564">
         <v>1.978</v>
       </c>
       <c r="H564">
-        <v>5.595</v>
+        <v>5.586</v>
       </c>
       <c r="I564">
         <v>0.14</v>
@@ -24914,13 +24914,13 @@
         <v>4.014</v>
       </c>
       <c r="L564">
-        <v>2.118</v>
+        <v>2.15</v>
       </c>
       <c r="M564">
-        <v>13.389</v>
+        <v>13.421</v>
       </c>
       <c r="N564">
-        <v>21.253</v>
+        <v>21.276</v>
       </c>
     </row>
     <row r="565" spans="1:14">
@@ -24931,40 +24931,40 @@
         <v>3.363</v>
       </c>
       <c r="C565">
-        <v>13.661</v>
+        <v>13.404</v>
       </c>
       <c r="D565">
-        <v>44.995</v>
+        <v>46.235</v>
       </c>
       <c r="E565">
-        <v>62.02</v>
-      </c>
-      <c r="F565" t="s">
-        <v>22</v>
+        <v>63.003</v>
+      </c>
+      <c r="F565">
+        <v>0.145</v>
       </c>
       <c r="G565">
-        <v>2.057</v>
+        <v>2.048</v>
       </c>
       <c r="H565">
-        <v>6.076</v>
+        <v>5.869</v>
       </c>
       <c r="I565">
-        <v>0.152</v>
+        <v>0.156</v>
       </c>
       <c r="J565">
         <v>7.284</v>
       </c>
       <c r="K565">
-        <v>3.574</v>
+        <v>3.725</v>
       </c>
       <c r="L565">
-        <v>1.96</v>
+        <v>1.993</v>
       </c>
       <c r="M565">
-        <v>12.817</v>
+        <v>13.002</v>
       </c>
       <c r="N565">
-        <v>21.279</v>
+        <v>21.22</v>
       </c>
     </row>
     <row r="566" spans="1:14">
@@ -24975,40 +24975,40 @@
         <v>3.038</v>
       </c>
       <c r="C566">
-        <v>14.884</v>
+        <v>14.571</v>
       </c>
       <c r="D566">
-        <v>40.641</v>
+        <v>41.761</v>
       </c>
       <c r="E566">
-        <v>58.563</v>
-      </c>
-      <c r="F566" t="s">
-        <v>22</v>
+        <v>59.37</v>
+      </c>
+      <c r="F566">
+        <v>0.132</v>
       </c>
       <c r="G566">
-        <v>1.882</v>
+        <v>1.873</v>
       </c>
       <c r="H566">
-        <v>6.503</v>
+        <v>6.319</v>
       </c>
       <c r="I566">
-        <v>0.14</v>
+        <v>0.138</v>
       </c>
       <c r="J566">
         <v>6.576</v>
       </c>
       <c r="K566">
-        <v>3.117</v>
+        <v>3.25</v>
       </c>
       <c r="L566">
-        <v>1.928</v>
+        <v>2.013</v>
       </c>
       <c r="M566">
-        <v>11.621</v>
+        <v>11.838</v>
       </c>
       <c r="N566">
-        <v>20.302</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="567" spans="1:14">
@@ -25019,40 +25019,40 @@
         <v>3.363</v>
       </c>
       <c r="C567">
-        <v>21.117</v>
+        <v>20.818</v>
       </c>
       <c r="D567">
-        <v>44.995</v>
+        <v>46.235</v>
       </c>
       <c r="E567">
-        <v>69.476</v>
-      </c>
-      <c r="F567" t="s">
-        <v>22</v>
+        <v>70.416</v>
+      </c>
+      <c r="F567">
+        <v>0.166</v>
       </c>
       <c r="G567">
-        <v>2.076</v>
+        <v>2.066</v>
       </c>
       <c r="H567">
-        <v>9.039</v>
+        <v>8.755</v>
       </c>
       <c r="I567">
-        <v>0.152</v>
+        <v>0.153</v>
       </c>
       <c r="J567">
         <v>7.196</v>
       </c>
       <c r="K567">
-        <v>3.342</v>
+        <v>3.465</v>
       </c>
       <c r="L567">
-        <v>2.114</v>
+        <v>2.119</v>
       </c>
       <c r="M567">
-        <v>12.652</v>
+        <v>12.781</v>
       </c>
       <c r="N567">
-        <v>24.101</v>
+        <v>23.922</v>
       </c>
     </row>
     <row r="568" spans="1:14">
@@ -25063,40 +25063,40 @@
         <v>3.255</v>
       </c>
       <c r="C568">
-        <v>23.699</v>
+        <v>23.285</v>
       </c>
       <c r="D568">
-        <v>43.544</v>
+        <v>44.744</v>
       </c>
       <c r="E568">
-        <v>70.497</v>
-      </c>
-      <c r="F568" t="s">
-        <v>22</v>
+        <v>71.283</v>
+      </c>
+      <c r="F568">
+        <v>0.17</v>
       </c>
       <c r="G568">
-        <v>1.865</v>
+        <v>1.859</v>
       </c>
       <c r="H568">
-        <v>10.032</v>
+        <v>9.674</v>
       </c>
       <c r="I568">
-        <v>0.169</v>
+        <v>0.154</v>
       </c>
       <c r="J568">
         <v>6.84</v>
       </c>
       <c r="K568">
-        <v>2.841</v>
+        <v>3.014</v>
       </c>
       <c r="L568">
-        <v>2.031</v>
+        <v>2.087</v>
       </c>
       <c r="M568">
-        <v>11.712</v>
+        <v>11.941</v>
       </c>
       <c r="N568">
-        <v>23.965</v>
+        <v>23.798</v>
       </c>
     </row>
     <row r="569" spans="1:14">
@@ -25107,40 +25107,40 @@
         <v>3.363</v>
       </c>
       <c r="C569">
-        <v>26.081</v>
+        <v>25.586</v>
       </c>
       <c r="D569">
-        <v>44.995</v>
+        <v>46.235</v>
       </c>
       <c r="E569">
-        <v>74.44</v>
-      </c>
-      <c r="F569" t="s">
-        <v>22</v>
+        <v>75.184</v>
+      </c>
+      <c r="F569">
+        <v>0.193</v>
       </c>
       <c r="G569">
-        <v>2.014</v>
+        <v>2.006</v>
       </c>
       <c r="H569">
-        <v>10.795</v>
+        <v>10.405</v>
       </c>
       <c r="I569">
-        <v>0.143</v>
+        <v>0.128</v>
       </c>
       <c r="J569">
         <v>7.062</v>
       </c>
       <c r="K569">
-        <v>2.617</v>
+        <v>2.933</v>
       </c>
       <c r="L569">
-        <v>2.229</v>
+        <v>2.294</v>
       </c>
       <c r="M569">
-        <v>11.908</v>
+        <v>12.289</v>
       </c>
       <c r="N569">
-        <v>25.091</v>
+        <v>25.021</v>
       </c>
     </row>
     <row r="570" spans="1:14">
@@ -25151,40 +25151,40 @@
         <v>3.255</v>
       </c>
       <c r="C570">
-        <v>26.608</v>
+        <v>26.096</v>
       </c>
       <c r="D570">
-        <v>43.544</v>
+        <v>44.744</v>
       </c>
       <c r="E570">
-        <v>73.407</v>
+        <v>74.094</v>
       </c>
       <c r="F570">
-        <v>0.188</v>
+        <v>0.162</v>
       </c>
       <c r="G570">
-        <v>1.929</v>
+        <v>1.921</v>
       </c>
       <c r="H570">
-        <v>10.919</v>
+        <v>10.521</v>
       </c>
       <c r="I570">
-        <v>0.127</v>
+        <v>0.109</v>
       </c>
       <c r="J570">
         <v>6.845</v>
       </c>
       <c r="K570">
-        <v>2.93</v>
+        <v>3.289</v>
       </c>
       <c r="L570">
-        <v>2.166</v>
+        <v>2.233</v>
       </c>
       <c r="M570">
-        <v>11.941</v>
+        <v>12.366</v>
       </c>
       <c r="N570">
-        <v>25.103</v>
+        <v>25.079</v>
       </c>
     </row>
     <row r="571" spans="1:14">
@@ -25195,40 +25195,40 @@
         <v>3.363</v>
       </c>
       <c r="C571">
-        <v>27.657</v>
+        <v>27.212</v>
       </c>
       <c r="D571">
-        <v>44.995</v>
+        <v>46.235</v>
       </c>
       <c r="E571">
-        <v>76.016</v>
-      </c>
-      <c r="F571" t="s">
-        <v>22</v>
+        <v>76.811</v>
+      </c>
+      <c r="F571">
+        <v>0.143</v>
       </c>
       <c r="G571">
-        <v>1.978</v>
+        <v>1.971</v>
       </c>
       <c r="H571">
-        <v>11.459</v>
+        <v>11.05</v>
       </c>
       <c r="I571">
-        <v>0.112</v>
+        <v>0.096</v>
       </c>
       <c r="J571">
         <v>7.193</v>
       </c>
       <c r="K571">
-        <v>2.898</v>
+        <v>3.189</v>
       </c>
       <c r="L571">
-        <v>2.16</v>
+        <v>2.24</v>
       </c>
       <c r="M571">
-        <v>12.25</v>
+        <v>12.622</v>
       </c>
       <c r="N571">
-        <v>25.954</v>
+        <v>25.881</v>
       </c>
     </row>
     <row r="572" spans="1:14">
@@ -25239,40 +25239,40 @@
         <v>3.363</v>
       </c>
       <c r="C572">
-        <v>26.6</v>
+        <v>26.19</v>
       </c>
       <c r="D572">
-        <v>44.995</v>
+        <v>46.235</v>
       </c>
       <c r="E572">
-        <v>74.958</v>
-      </c>
-      <c r="F572" t="s">
-        <v>22</v>
+        <v>75.788</v>
+      </c>
+      <c r="F572">
+        <v>0.134</v>
       </c>
       <c r="G572">
-        <v>1.953</v>
+        <v>1.947</v>
       </c>
       <c r="H572">
-        <v>10.912</v>
+        <v>10.512</v>
       </c>
       <c r="I572">
-        <v>0.098</v>
+        <v>0.084</v>
       </c>
       <c r="J572">
         <v>7.149</v>
       </c>
       <c r="K572">
-        <v>3.019</v>
+        <v>3.347</v>
       </c>
       <c r="L572">
-        <v>2.198</v>
+        <v>2.222</v>
       </c>
       <c r="M572">
-        <v>12.365</v>
+        <v>12.719</v>
       </c>
       <c r="N572">
-        <v>25.475</v>
+        <v>25.395</v>
       </c>
     </row>
     <row r="573" spans="1:14">
@@ -25283,22 +25283,22 @@
         <v>3.255</v>
       </c>
       <c r="C573">
-        <v>23.527</v>
+        <v>23.163</v>
       </c>
       <c r="D573">
-        <v>43.544</v>
+        <v>44.744</v>
       </c>
       <c r="E573">
-        <v>70.325</v>
-      </c>
-      <c r="F573" t="s">
-        <v>22</v>
+        <v>71.161</v>
+      </c>
+      <c r="F573">
+        <v>0.106</v>
       </c>
       <c r="G573">
-        <v>1.888</v>
+        <v>1.882</v>
       </c>
       <c r="H573">
-        <v>9.698</v>
+        <v>9.346</v>
       </c>
       <c r="I573">
         <v>0.123</v>
@@ -25307,16 +25307,16 @@
         <v>6.918</v>
       </c>
       <c r="K573">
-        <v>2.895</v>
+        <v>3.207</v>
       </c>
       <c r="L573">
-        <v>2.014</v>
+        <v>2.074</v>
       </c>
       <c r="M573">
-        <v>11.826</v>
+        <v>12.199</v>
       </c>
       <c r="N573">
-        <v>23.648</v>
+        <v>23.656</v>
       </c>
     </row>
     <row r="574" spans="1:14">
@@ -25327,40 +25327,1096 @@
         <v>3.363</v>
       </c>
       <c r="C574">
-        <v>20.788</v>
+        <v>20.399</v>
       </c>
       <c r="D574">
-        <v>44.995</v>
+        <v>46.235</v>
       </c>
       <c r="E574">
-        <v>69.147</v>
-      </c>
-      <c r="F574" t="s">
-        <v>22</v>
+        <v>69.997</v>
+      </c>
+      <c r="F574">
+        <v>0.096</v>
       </c>
       <c r="G574">
-        <v>2.021</v>
+        <v>2.013</v>
       </c>
       <c r="H574">
-        <v>8.554</v>
+        <v>8.255</v>
       </c>
       <c r="I574">
-        <v>0.149</v>
+        <v>0.153</v>
       </c>
       <c r="J574">
         <v>7.152</v>
       </c>
       <c r="K574">
-        <v>3.028</v>
+        <v>3.179</v>
       </c>
       <c r="L574">
-        <v>2.192</v>
+        <v>2.258</v>
       </c>
       <c r="M574">
-        <v>12.373</v>
+        <v>12.589</v>
       </c>
       <c r="N574">
-        <v>23.205</v>
+        <v>23.106</v>
+      </c>
+    </row>
+    <row r="575" spans="1:14">
+      <c r="A575" s="6">
+        <v>43770</v>
+      </c>
+      <c r="B575">
+        <v>3.255</v>
+      </c>
+      <c r="C575">
+        <v>16.144</v>
+      </c>
+      <c r="D575">
+        <v>44.744</v>
+      </c>
+      <c r="E575">
+        <v>64.142</v>
+      </c>
+      <c r="F575">
+        <v>0.109</v>
+      </c>
+      <c r="G575">
+        <v>1.995</v>
+      </c>
+      <c r="H575">
+        <v>6.401</v>
+      </c>
+      <c r="I575">
+        <v>0.147</v>
+      </c>
+      <c r="J575">
+        <v>6.949</v>
+      </c>
+      <c r="K575">
+        <v>3.115</v>
+      </c>
+      <c r="L575">
+        <v>2.203</v>
+      </c>
+      <c r="M575">
+        <v>12.268</v>
+      </c>
+      <c r="N575">
+        <v>20.92</v>
+      </c>
+    </row>
+    <row r="576" spans="1:14">
+      <c r="A576" s="6">
+        <v>43800</v>
+      </c>
+      <c r="B576">
+        <v>3.363</v>
+      </c>
+      <c r="C576">
+        <v>14.594</v>
+      </c>
+      <c r="D576">
+        <v>46.235</v>
+      </c>
+      <c r="E576">
+        <v>64.192</v>
+      </c>
+      <c r="F576">
+        <v>0.121</v>
+      </c>
+      <c r="G576">
+        <v>2.053</v>
+      </c>
+      <c r="H576">
+        <v>6.088</v>
+      </c>
+      <c r="I576">
+        <v>0.152</v>
+      </c>
+      <c r="J576">
+        <v>7.135</v>
+      </c>
+      <c r="K576">
+        <v>3.328</v>
+      </c>
+      <c r="L576">
+        <v>2.194</v>
+      </c>
+      <c r="M576">
+        <v>12.657</v>
+      </c>
+      <c r="N576">
+        <v>21.071</v>
+      </c>
+    </row>
+    <row r="577" spans="1:14">
+      <c r="A577" s="6">
+        <v>43831</v>
+      </c>
+      <c r="B577">
+        <v>3.354</v>
+      </c>
+      <c r="C577">
+        <v>15.735</v>
+      </c>
+      <c r="D577">
+        <v>38.751</v>
+      </c>
+      <c r="E577">
+        <v>57.84</v>
+      </c>
+      <c r="F577">
+        <v>0.155</v>
+      </c>
+      <c r="G577">
+        <v>1.979</v>
+      </c>
+      <c r="H577">
+        <v>6.73</v>
+      </c>
+      <c r="I577">
+        <v>0.136</v>
+      </c>
+      <c r="J577">
+        <v>7.202</v>
+      </c>
+      <c r="K577">
+        <v>3.309</v>
+      </c>
+      <c r="L577">
+        <v>2.135</v>
+      </c>
+      <c r="M577">
+        <v>12.646</v>
+      </c>
+      <c r="N577">
+        <v>21.646</v>
+      </c>
+    </row>
+    <row r="578" spans="1:14">
+      <c r="A578" s="6">
+        <v>43862</v>
+      </c>
+      <c r="B578">
+        <v>3.138</v>
+      </c>
+      <c r="C578">
+        <v>17.904</v>
+      </c>
+      <c r="D578">
+        <v>36.251</v>
+      </c>
+      <c r="E578">
+        <v>57.292</v>
+      </c>
+      <c r="F578">
+        <v>0.16</v>
+      </c>
+      <c r="G578">
+        <v>1.921</v>
+      </c>
+      <c r="H578">
+        <v>7.637</v>
+      </c>
+      <c r="I578">
+        <v>0.143</v>
+      </c>
+      <c r="J578">
+        <v>6.734</v>
+      </c>
+      <c r="K578">
+        <v>3.042</v>
+      </c>
+      <c r="L578">
+        <v>1.959</v>
+      </c>
+      <c r="M578">
+        <v>11.736</v>
+      </c>
+      <c r="N578">
+        <v>21.596</v>
+      </c>
+    </row>
+    <row r="579" spans="1:14">
+      <c r="A579" s="6">
+        <v>43891</v>
+      </c>
+      <c r="B579">
+        <v>3.354</v>
+      </c>
+      <c r="C579">
+        <v>23.28</v>
+      </c>
+      <c r="D579">
+        <v>38.751</v>
+      </c>
+      <c r="E579">
+        <v>65.385</v>
+      </c>
+      <c r="F579">
+        <v>0.147</v>
+      </c>
+      <c r="G579">
+        <v>2.047</v>
+      </c>
+      <c r="H579">
+        <v>9.896</v>
+      </c>
+      <c r="I579">
+        <v>0.15</v>
+      </c>
+      <c r="J579">
+        <v>7.055</v>
+      </c>
+      <c r="K579">
+        <v>3.357</v>
+      </c>
+      <c r="L579">
+        <v>1.708</v>
+      </c>
+      <c r="M579">
+        <v>12.121</v>
+      </c>
+      <c r="N579">
+        <v>24.36</v>
+      </c>
+    </row>
+    <row r="580" spans="1:14">
+      <c r="A580" s="6">
+        <v>43922</v>
+      </c>
+      <c r="B580">
+        <v>3.246</v>
+      </c>
+      <c r="C580">
+        <v>26.177</v>
+      </c>
+      <c r="D580">
+        <v>37.501</v>
+      </c>
+      <c r="E580">
+        <v>66.924</v>
+      </c>
+      <c r="F580">
+        <v>0.149</v>
+      </c>
+      <c r="G580">
+        <v>1.961</v>
+      </c>
+      <c r="H580">
+        <v>10.911</v>
+      </c>
+      <c r="I580">
+        <v>0.154</v>
+      </c>
+      <c r="J580">
+        <v>6.7</v>
+      </c>
+      <c r="K580">
+        <v>3.099</v>
+      </c>
+      <c r="L580">
+        <v>1.21</v>
+      </c>
+      <c r="M580">
+        <v>11.009</v>
+      </c>
+      <c r="N580">
+        <v>24.184</v>
+      </c>
+    </row>
+    <row r="581" spans="1:14">
+      <c r="A581" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B581">
+        <v>3.354</v>
+      </c>
+      <c r="C581">
+        <v>29.504</v>
+      </c>
+      <c r="D581">
+        <v>38.751</v>
+      </c>
+      <c r="E581">
+        <v>71.609</v>
+      </c>
+      <c r="F581">
+        <v>0.202</v>
+      </c>
+      <c r="G581">
+        <v>2.008</v>
+      </c>
+      <c r="H581">
+        <v>12.061</v>
+      </c>
+      <c r="I581">
+        <v>0.131</v>
+      </c>
+      <c r="J581">
+        <v>7.021</v>
+      </c>
+      <c r="K581">
+        <v>3.22</v>
+      </c>
+      <c r="L581">
+        <v>1.748</v>
+      </c>
+      <c r="M581">
+        <v>11.989</v>
+      </c>
+      <c r="N581">
+        <v>26.39</v>
+      </c>
+    </row>
+    <row r="582" spans="1:14">
+      <c r="A582" s="6">
+        <v>43983</v>
+      </c>
+      <c r="B582">
+        <v>3.246</v>
+      </c>
+      <c r="C582">
+        <v>29.507</v>
+      </c>
+      <c r="D582">
+        <v>37.501</v>
+      </c>
+      <c r="E582">
+        <v>70.254</v>
+      </c>
+      <c r="F582">
+        <v>0.192</v>
+      </c>
+      <c r="G582">
+        <v>1.91</v>
+      </c>
+      <c r="H582">
+        <v>12.029</v>
+      </c>
+      <c r="I582">
+        <v>0.131</v>
+      </c>
+      <c r="J582">
+        <v>6.903</v>
+      </c>
+      <c r="K582">
+        <v>3.051</v>
+      </c>
+      <c r="L582">
+        <v>2.015</v>
+      </c>
+      <c r="M582">
+        <v>11.969</v>
+      </c>
+      <c r="N582">
+        <v>26.232</v>
+      </c>
+    </row>
+    <row r="583" spans="1:14">
+      <c r="A583" s="6">
+        <v>44013</v>
+      </c>
+      <c r="B583">
+        <v>3.354</v>
+      </c>
+      <c r="C583">
+        <v>30.337</v>
+      </c>
+      <c r="D583">
+        <v>38.751</v>
+      </c>
+      <c r="E583">
+        <v>72.442</v>
+      </c>
+      <c r="F583">
+        <v>0.183</v>
+      </c>
+      <c r="G583">
+        <v>1.935</v>
+      </c>
+      <c r="H583">
+        <v>12.497</v>
+      </c>
+      <c r="I583">
+        <v>0.089</v>
+      </c>
+      <c r="J583">
+        <v>7.009</v>
+      </c>
+      <c r="K583">
+        <v>3.265</v>
+      </c>
+      <c r="L583">
+        <v>2.01</v>
+      </c>
+      <c r="M583">
+        <v>12.284</v>
+      </c>
+      <c r="N583">
+        <v>26.988</v>
+      </c>
+    </row>
+    <row r="584" spans="1:14">
+      <c r="A584" s="6">
+        <v>44044</v>
+      </c>
+      <c r="B584">
+        <v>3.354</v>
+      </c>
+      <c r="C584">
+        <v>28.786</v>
+      </c>
+      <c r="D584">
+        <v>38.751</v>
+      </c>
+      <c r="E584">
+        <v>70.891</v>
+      </c>
+      <c r="F584">
+        <v>0.158</v>
+      </c>
+      <c r="G584">
+        <v>1.934</v>
+      </c>
+      <c r="H584">
+        <v>11.927</v>
+      </c>
+      <c r="I584">
+        <v>0.099</v>
+      </c>
+      <c r="J584">
+        <v>7.004</v>
+      </c>
+      <c r="K584">
+        <v>3.261</v>
+      </c>
+      <c r="L584">
+        <v>1.988</v>
+      </c>
+      <c r="M584">
+        <v>12.252</v>
+      </c>
+      <c r="N584">
+        <v>26.37</v>
+      </c>
+    </row>
+    <row r="585" spans="1:14">
+      <c r="A585" s="6">
+        <v>44075</v>
+      </c>
+      <c r="B585">
+        <v>3.246</v>
+      </c>
+      <c r="C585">
+        <v>25.431</v>
+      </c>
+      <c r="D585">
+        <v>37.501</v>
+      </c>
+      <c r="E585">
+        <v>66.178</v>
+      </c>
+      <c r="F585">
+        <v>0.127</v>
+      </c>
+      <c r="G585">
+        <v>1.91</v>
+      </c>
+      <c r="H585">
+        <v>10.609</v>
+      </c>
+      <c r="I585">
+        <v>0.107</v>
+      </c>
+      <c r="J585">
+        <v>6.665</v>
+      </c>
+      <c r="K585">
+        <v>3.069</v>
+      </c>
+      <c r="L585">
+        <v>1.972</v>
+      </c>
+      <c r="M585">
+        <v>11.706</v>
+      </c>
+      <c r="N585">
+        <v>24.46</v>
+      </c>
+    </row>
+    <row r="586" spans="1:14">
+      <c r="A586" s="6">
+        <v>44105</v>
+      </c>
+      <c r="B586">
+        <v>3.354</v>
+      </c>
+      <c r="C586">
+        <v>22.877</v>
+      </c>
+      <c r="D586">
+        <v>38.751</v>
+      </c>
+      <c r="E586">
+        <v>64.982</v>
+      </c>
+      <c r="F586">
+        <v>0.125</v>
+      </c>
+      <c r="G586">
+        <v>2.006</v>
+      </c>
+      <c r="H586">
+        <v>9.251</v>
+      </c>
+      <c r="I586">
+        <v>0.106</v>
+      </c>
+      <c r="J586">
+        <v>6.919</v>
+      </c>
+      <c r="K586">
+        <v>3.096</v>
+      </c>
+      <c r="L586">
+        <v>1.894</v>
+      </c>
+      <c r="M586">
+        <v>11.908</v>
+      </c>
+      <c r="N586">
+        <v>23.396</v>
+      </c>
+    </row>
+    <row r="587" spans="1:14">
+      <c r="A587" s="6">
+        <v>44136</v>
+      </c>
+      <c r="B587">
+        <v>3.246</v>
+      </c>
+      <c r="C587">
+        <v>18.817</v>
+      </c>
+      <c r="D587">
+        <v>37.501</v>
+      </c>
+      <c r="E587">
+        <v>59.564</v>
+      </c>
+      <c r="F587">
+        <v>0.135</v>
+      </c>
+      <c r="G587">
+        <v>1.973</v>
+      </c>
+      <c r="H587">
+        <v>7.369</v>
+      </c>
+      <c r="I587">
+        <v>0.122</v>
+      </c>
+      <c r="J587">
+        <v>6.737</v>
+      </c>
+      <c r="K587">
+        <v>3.022</v>
+      </c>
+      <c r="L587">
+        <v>1.944</v>
+      </c>
+      <c r="M587">
+        <v>11.703</v>
+      </c>
+      <c r="N587">
+        <v>21.302</v>
+      </c>
+    </row>
+    <row r="588" spans="1:14">
+      <c r="A588" s="6">
+        <v>44166</v>
+      </c>
+      <c r="B588">
+        <v>3.354</v>
+      </c>
+      <c r="C588">
+        <v>17.175</v>
+      </c>
+      <c r="D588">
+        <v>38.751</v>
+      </c>
+      <c r="E588">
+        <v>59.28</v>
+      </c>
+      <c r="F588">
+        <v>0.141</v>
+      </c>
+      <c r="G588">
+        <v>2.055</v>
+      </c>
+      <c r="H588">
+        <v>7.038</v>
+      </c>
+      <c r="I588">
+        <v>0.105</v>
+      </c>
+      <c r="J588">
+        <v>7.002</v>
+      </c>
+      <c r="K588">
+        <v>3.061</v>
+      </c>
+      <c r="L588">
+        <v>1.978</v>
+      </c>
+      <c r="M588">
+        <v>12.042</v>
+      </c>
+      <c r="N588">
+        <v>21.381</v>
+      </c>
+    </row>
+    <row r="589" spans="1:14">
+      <c r="A589" s="6">
+        <v>44197</v>
+      </c>
+      <c r="B589">
+        <v>3.363</v>
+      </c>
+      <c r="C589">
+        <v>18.223</v>
+      </c>
+      <c r="D589">
+        <v>38.587</v>
+      </c>
+      <c r="E589">
+        <v>60.173</v>
+      </c>
+      <c r="F589">
+        <v>0.193</v>
+      </c>
+      <c r="G589">
+        <v>2.059</v>
+      </c>
+      <c r="H589">
+        <v>7.838</v>
+      </c>
+      <c r="I589">
+        <v>0.125</v>
+      </c>
+      <c r="J589">
+        <v>6.982</v>
+      </c>
+      <c r="K589">
+        <v>3.238</v>
+      </c>
+      <c r="L589">
+        <v>1.757</v>
+      </c>
+      <c r="M589">
+        <v>11.977</v>
+      </c>
+      <c r="N589">
+        <v>22.192</v>
+      </c>
+    </row>
+    <row r="590" spans="1:14">
+      <c r="A590" s="6">
+        <v>44228</v>
+      </c>
+      <c r="B590">
+        <v>3.038</v>
+      </c>
+      <c r="C590">
+        <v>19.589</v>
+      </c>
+      <c r="D590">
+        <v>34.853</v>
+      </c>
+      <c r="E590">
+        <v>57.48</v>
+      </c>
+      <c r="F590">
+        <v>0.165</v>
+      </c>
+      <c r="G590">
+        <v>1.857</v>
+      </c>
+      <c r="H590">
+        <v>8.464</v>
+      </c>
+      <c r="I590">
+        <v>0.121</v>
+      </c>
+      <c r="J590">
+        <v>6.451</v>
+      </c>
+      <c r="K590">
+        <v>2.657</v>
+      </c>
+      <c r="L590">
+        <v>1.634</v>
+      </c>
+      <c r="M590">
+        <v>10.743</v>
+      </c>
+      <c r="N590">
+        <v>21.349</v>
+      </c>
+    </row>
+    <row r="591" spans="1:14">
+      <c r="A591" s="6">
+        <v>44256</v>
+      </c>
+      <c r="B591">
+        <v>3.363</v>
+      </c>
+      <c r="C591">
+        <v>27.1</v>
+      </c>
+      <c r="D591">
+        <v>38.587</v>
+      </c>
+      <c r="E591">
+        <v>69.05</v>
+      </c>
+      <c r="F591" t="s">
+        <v>22</v>
+      </c>
+      <c r="G591">
+        <v>1.824</v>
+      </c>
+      <c r="H591">
+        <v>11.674</v>
+      </c>
+      <c r="I591">
+        <v>0.17</v>
+      </c>
+      <c r="J591">
+        <v>6.97</v>
+      </c>
+      <c r="K591">
+        <v>3.07</v>
+      </c>
+      <c r="L591">
+        <v>2.095</v>
+      </c>
+      <c r="M591">
+        <v>12.136</v>
+      </c>
+      <c r="N591">
+        <v>25.953</v>
+      </c>
+    </row>
+    <row r="592" spans="1:14">
+      <c r="A592" s="6">
+        <v>44287</v>
+      </c>
+      <c r="B592">
+        <v>3.255</v>
+      </c>
+      <c r="C592">
+        <v>30.646</v>
+      </c>
+      <c r="D592">
+        <v>37.343</v>
+      </c>
+      <c r="E592">
+        <v>71.243</v>
+      </c>
+      <c r="F592">
+        <v>0.14</v>
+      </c>
+      <c r="G592">
+        <v>1.947</v>
+      </c>
+      <c r="H592">
+        <v>12.971</v>
+      </c>
+      <c r="I592">
+        <v>0.145</v>
+      </c>
+      <c r="J592">
+        <v>6.682</v>
+      </c>
+      <c r="K592">
+        <v>2.852</v>
+      </c>
+      <c r="L592">
+        <v>1.945</v>
+      </c>
+      <c r="M592">
+        <v>11.479</v>
+      </c>
+      <c r="N592">
+        <v>26.682</v>
+      </c>
+    </row>
+    <row r="593" spans="1:14">
+      <c r="A593" s="6">
+        <v>44317</v>
+      </c>
+      <c r="B593">
+        <v>3.363</v>
+      </c>
+      <c r="C593">
+        <v>33.959</v>
+      </c>
+      <c r="D593">
+        <v>38.587</v>
+      </c>
+      <c r="E593">
+        <v>75.91</v>
+      </c>
+      <c r="F593" t="s">
+        <v>22</v>
+      </c>
+      <c r="G593">
+        <v>2.121</v>
+      </c>
+      <c r="H593">
+        <v>14.056</v>
+      </c>
+      <c r="I593">
+        <v>0.124</v>
+      </c>
+      <c r="J593">
+        <v>6.857</v>
+      </c>
+      <c r="K593">
+        <v>2.733</v>
+      </c>
+      <c r="L593">
+        <v>2.234</v>
+      </c>
+      <c r="M593">
+        <v>11.823</v>
+      </c>
+      <c r="N593">
+        <v>28.286</v>
+      </c>
+    </row>
+    <row r="594" spans="1:14">
+      <c r="A594" s="6">
+        <v>44348</v>
+      </c>
+      <c r="B594">
+        <v>3.255</v>
+      </c>
+      <c r="C594">
+        <v>34.39</v>
+      </c>
+      <c r="D594">
+        <v>37.343</v>
+      </c>
+      <c r="E594">
+        <v>74.987</v>
+      </c>
+      <c r="F594" t="s">
+        <v>22</v>
+      </c>
+      <c r="G594">
+        <v>1.973</v>
+      </c>
+      <c r="H594">
+        <v>14.151</v>
+      </c>
+      <c r="I594">
+        <v>0.106</v>
+      </c>
+      <c r="J594">
+        <v>6.844</v>
+      </c>
+      <c r="K594">
+        <v>2.73</v>
+      </c>
+      <c r="L594">
+        <v>2.173</v>
+      </c>
+      <c r="M594">
+        <v>11.748</v>
+      </c>
+      <c r="N594">
+        <v>28.153</v>
+      </c>
+    </row>
+    <row r="595" spans="1:14">
+      <c r="A595" s="6">
+        <v>44378</v>
+      </c>
+      <c r="B595">
+        <v>3.363</v>
+      </c>
+      <c r="C595">
+        <v>34.925</v>
+      </c>
+      <c r="D595">
+        <v>38.587</v>
+      </c>
+      <c r="E595">
+        <v>76.875</v>
+      </c>
+      <c r="F595" t="s">
+        <v>22</v>
+      </c>
+      <c r="G595">
+        <v>2.018</v>
+      </c>
+      <c r="H595">
+        <v>14.636</v>
+      </c>
+      <c r="I595">
+        <v>0.077</v>
+      </c>
+      <c r="J595">
+        <v>7.106</v>
+      </c>
+      <c r="K595">
+        <v>3.094</v>
+      </c>
+      <c r="L595">
+        <v>2.232</v>
+      </c>
+      <c r="M595">
+        <v>12.432</v>
+      </c>
+      <c r="N595">
+        <v>29.318</v>
+      </c>
+    </row>
+    <row r="596" spans="1:14">
+      <c r="A596" s="6">
+        <v>44409</v>
+      </c>
+      <c r="B596">
+        <v>3.363</v>
+      </c>
+      <c r="C596">
+        <v>32.935</v>
+      </c>
+      <c r="D596">
+        <v>38.587</v>
+      </c>
+      <c r="E596">
+        <v>74.886</v>
+      </c>
+      <c r="F596" t="s">
+        <v>22</v>
+      </c>
+      <c r="G596">
+        <v>2.037</v>
+      </c>
+      <c r="H596">
+        <v>14.063</v>
+      </c>
+      <c r="I596">
+        <v>0.104</v>
+      </c>
+      <c r="J596">
+        <v>7.112</v>
+      </c>
+      <c r="K596">
+        <v>3.042</v>
+      </c>
+      <c r="L596">
+        <v>2.168</v>
+      </c>
+      <c r="M596">
+        <v>12.322</v>
+      </c>
+      <c r="N596">
+        <v>28.67</v>
+      </c>
+    </row>
+    <row r="597" spans="1:14">
+      <c r="A597" s="6">
+        <v>44440</v>
+      </c>
+      <c r="B597">
+        <v>3.255</v>
+      </c>
+      <c r="C597">
+        <v>29.157</v>
+      </c>
+      <c r="D597">
+        <v>37.343</v>
+      </c>
+      <c r="E597">
+        <v>69.754</v>
+      </c>
+      <c r="F597">
+        <v>0.119</v>
+      </c>
+      <c r="G597">
+        <v>1.995</v>
+      </c>
+      <c r="H597">
+        <v>12.569</v>
+      </c>
+      <c r="I597">
+        <v>0.114</v>
+      </c>
+      <c r="J597">
+        <v>6.877</v>
+      </c>
+      <c r="K597">
+        <v>2.901</v>
+      </c>
+      <c r="L597">
+        <v>2.052</v>
+      </c>
+      <c r="M597">
+        <v>11.829</v>
+      </c>
+      <c r="N597">
+        <v>26.626</v>
+      </c>
+    </row>
+    <row r="598" spans="1:14">
+      <c r="A598" s="6">
+        <v>44470</v>
+      </c>
+      <c r="B598">
+        <v>3.363</v>
+      </c>
+      <c r="C598">
+        <v>25.897</v>
+      </c>
+      <c r="D598">
+        <v>38.587</v>
+      </c>
+      <c r="E598">
+        <v>67.848</v>
+      </c>
+      <c r="F598" t="s">
+        <v>22</v>
+      </c>
+      <c r="G598">
+        <v>2.097</v>
+      </c>
+      <c r="H598">
+        <v>10.966</v>
+      </c>
+      <c r="I598">
+        <v>0.131</v>
+      </c>
+      <c r="J598">
+        <v>6.98</v>
+      </c>
+      <c r="K598">
+        <v>2.795</v>
+      </c>
+      <c r="L598">
+        <v>2.25</v>
+      </c>
+      <c r="M598">
+        <v>12.025</v>
+      </c>
+      <c r="N598">
+        <v>25.331</v>
       </c>
     </row>
   </sheetData>
@@ -25387,7 +26443,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N82"/>
+  <dimension ref="A1:N84"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -28396,13 +29452,13 @@
         <v>39.6</v>
       </c>
       <c r="C78">
-        <v>109.399</v>
+        <v>109.407</v>
       </c>
       <c r="D78">
         <v>578.535</v>
       </c>
       <c r="E78">
-        <v>727.534</v>
+        <v>727.542</v>
       </c>
       <c r="F78">
         <v>0.365</v>
@@ -28440,13 +29496,13 @@
         <v>39.6</v>
       </c>
       <c r="C79">
-        <v>128.099</v>
+        <v>128.213</v>
       </c>
       <c r="D79">
         <v>512.736</v>
       </c>
       <c r="E79">
-        <v>680.435</v>
+        <v>680.549</v>
       </c>
       <c r="F79">
         <v>0.325</v>
@@ -28484,13 +29540,13 @@
         <v>39.6</v>
       </c>
       <c r="C80">
-        <v>161.293</v>
+        <v>161.502</v>
       </c>
       <c r="D80">
-        <v>447.84</v>
+        <v>444.555</v>
       </c>
       <c r="E80">
-        <v>648.733</v>
+        <v>645.657</v>
       </c>
       <c r="F80">
         <v>2.004</v>
@@ -28528,13 +29584,13 @@
         <v>39.6</v>
       </c>
       <c r="C81">
-        <v>193.384</v>
+        <v>193.414</v>
       </c>
       <c r="D81">
-        <v>432.991</v>
+        <v>429.198</v>
       </c>
       <c r="E81">
-        <v>665.975</v>
+        <v>662.212</v>
       </c>
       <c r="F81">
         <v>2.208</v>
@@ -28572,25 +29628,25 @@
         <v>39.6</v>
       </c>
       <c r="C82">
-        <v>221.512</v>
+        <v>220.837</v>
       </c>
       <c r="D82">
-        <v>517.237</v>
+        <v>524.353</v>
       </c>
       <c r="E82">
-        <v>778.349</v>
+        <v>784.79</v>
       </c>
       <c r="F82">
-        <v>2.073</v>
+        <v>2.069</v>
       </c>
       <c r="G82">
-        <v>20.005</v>
+        <v>20.004</v>
       </c>
       <c r="H82">
-        <v>94.13</v>
+        <v>93.985</v>
       </c>
       <c r="I82">
-        <v>1.588</v>
+        <v>1.585</v>
       </c>
       <c r="J82">
         <v>84.073</v>
@@ -28599,13 +29655,101 @@
         <v>46.924</v>
       </c>
       <c r="L82">
-        <v>25.097</v>
+        <v>25.477</v>
       </c>
       <c r="M82">
-        <v>156.095</v>
+        <v>156.474</v>
       </c>
       <c r="N82">
-        <v>273.889</v>
+        <v>274.119</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="A83" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B83">
+        <v>39.6</v>
+      </c>
+      <c r="C83">
+        <v>251.461</v>
+      </c>
+      <c r="D83">
+        <v>544.381</v>
+      </c>
+      <c r="E83">
+        <v>835.442</v>
+      </c>
+      <c r="F83">
+        <v>1.677</v>
+      </c>
+      <c r="G83">
+        <v>23.634</v>
+      </c>
+      <c r="H83">
+        <v>103.195</v>
+      </c>
+      <c r="I83">
+        <v>1.592</v>
+      </c>
+      <c r="J83">
+        <v>84.299</v>
+      </c>
+      <c r="K83">
+        <v>39.04</v>
+      </c>
+      <c r="L83">
+        <v>25.932</v>
+      </c>
+      <c r="M83">
+        <v>149.271</v>
+      </c>
+      <c r="N83">
+        <v>279.369</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
+      <c r="A84" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B84">
+        <v>39.6</v>
+      </c>
+      <c r="C84">
+        <v>285.529</v>
+      </c>
+      <c r="D84">
+        <v>457.513</v>
+      </c>
+      <c r="E84">
+        <v>782.642</v>
+      </c>
+      <c r="F84">
+        <v>1.874</v>
+      </c>
+      <c r="G84">
+        <v>23.639</v>
+      </c>
+      <c r="H84">
+        <v>117.955</v>
+      </c>
+      <c r="I84">
+        <v>1.473</v>
+      </c>
+      <c r="J84">
+        <v>82.95</v>
+      </c>
+      <c r="K84">
+        <v>37.854</v>
+      </c>
+      <c r="L84">
+        <v>22.562</v>
+      </c>
+      <c r="M84">
+        <v>143.366</v>
+      </c>
+      <c r="N84">
+        <v>288.308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>